<commit_message>
Updated the RMM Matrix
- Documented the new raspberry pi overheating risk and mitigation plan
</commit_message>
<xml_diff>
--- a/Documentation/Home_Automation_RMM.xlsx
+++ b/Documentation/Home_Automation_RMM.xlsx
@@ -4,12 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="0" windowWidth="21560" windowHeight="20300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19040" windowHeight="16220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -321,7 +319,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M9" authorId="0">
+    <comment ref="M10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -350,7 +348,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Number</t>
   </si>
@@ -431,6 +429,15 @@
   </si>
   <si>
     <t>Totals (Hours)</t>
+  </si>
+  <si>
+    <t>R-004</t>
+  </si>
+  <si>
+    <t>Due to the design of the physical model, the raspberry pi devices that will be housed in the attic may suffer form excessive heat build up and cause degraded performance.</t>
+  </si>
+  <si>
+    <t>1. Install a cooling fan in the attic to reduce the heat build-up in addition to a heat extractor vent that can help cool the system.</t>
   </si>
 </sst>
 </file>
@@ -1072,13 +1079,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y137"/>
+  <dimension ref="A1:Y138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1389,20 +1396,49 @@
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
     </row>
-    <row r="8" spans="1:25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="5"/>
+    <row r="8" spans="1:25" ht="121">
+      <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="6">
+        <v>43169</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0.35</v>
+      </c>
+      <c r="F8" s="4">
+        <v>16</v>
+      </c>
+      <c r="G8" s="4">
+        <f>E8*F8</f>
+        <v>5.6</v>
+      </c>
+      <c r="H8" s="6">
+        <v>43173</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="13">
+        <v>16</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="L8" s="4">
+        <f>K8*F8</f>
+        <v>1.6</v>
+      </c>
+      <c r="M8" s="5">
+        <f>J8+L8</f>
+        <v>17.600000000000001</v>
+      </c>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
@@ -1416,76 +1452,76 @@
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
     </row>
-    <row r="9" spans="1:25" s="11" customFormat="1" ht="25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8" t="s">
+    <row r="9" spans="1:25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+    </row>
+    <row r="10" spans="1:25" s="11" customFormat="1" ht="25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F10" s="9">
         <f>SUM(F3:F7)</f>
         <v>40.5</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G10" s="9">
         <f>SUM(G3:G7)</f>
         <v>20.125</v>
       </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9">
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9">
         <f>SUM(J3:J7)</f>
         <v>25</v>
       </c>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9">
+      <c r="K10" s="9"/>
+      <c r="L10" s="9">
         <f>SUM(L3:L7)</f>
         <v>5.65</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M10" s="9">
         <f>SUM(M3:M7)</f>
         <v>30.65</v>
       </c>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="10"/>
-    </row>
-    <row r="10" spans="1:25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
     </row>
     <row r="11" spans="1:25">
       <c r="A11" s="4"/>
@@ -4593,18 +4629,18 @@
       <c r="Y125" s="5"/>
     </row>
     <row r="126" spans="1:25">
-      <c r="A126" s="5"/>
-      <c r="B126" s="5"/>
-      <c r="C126" s="5"/>
-      <c r="D126" s="5"/>
-      <c r="E126" s="5"/>
-      <c r="F126" s="5"/>
-      <c r="G126" s="5"/>
-      <c r="H126" s="5"/>
-      <c r="I126" s="5"/>
-      <c r="J126" s="5"/>
-      <c r="K126" s="5"/>
-      <c r="L126" s="5"/>
+      <c r="A126" s="4"/>
+      <c r="B126" s="4"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="4"/>
+      <c r="E126" s="4"/>
+      <c r="F126" s="4"/>
+      <c r="G126" s="4"/>
+      <c r="H126" s="4"/>
+      <c r="I126" s="4"/>
+      <c r="J126" s="4"/>
+      <c r="K126" s="4"/>
+      <c r="L126" s="4"/>
       <c r="M126" s="5"/>
       <c r="N126" s="5"/>
       <c r="O126" s="5"/>
@@ -4916,6 +4952,33 @@
       <c r="X137" s="5"/>
       <c r="Y137" s="5"/>
     </row>
+    <row r="138" spans="1:25">
+      <c r="A138" s="5"/>
+      <c r="B138" s="5"/>
+      <c r="C138" s="5"/>
+      <c r="D138" s="5"/>
+      <c r="E138" s="5"/>
+      <c r="F138" s="5"/>
+      <c r="G138" s="5"/>
+      <c r="H138" s="5"/>
+      <c r="I138" s="5"/>
+      <c r="J138" s="5"/>
+      <c r="K138" s="5"/>
+      <c r="L138" s="5"/>
+      <c r="M138" s="5"/>
+      <c r="N138" s="5"/>
+      <c r="O138" s="5"/>
+      <c r="P138" s="5"/>
+      <c r="Q138" s="5"/>
+      <c r="R138" s="5"/>
+      <c r="S138" s="5"/>
+      <c r="T138" s="5"/>
+      <c r="U138" s="5"/>
+      <c r="V138" s="5"/>
+      <c r="W138" s="5"/>
+      <c r="X138" s="5"/>
+      <c r="Y138" s="5"/>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
@@ -4928,44 +4991,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter alignWithMargins="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter alignWithMargins="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added "Wiring Risk" to RMM
- Added the risk of soldering the wires to button up the safety of the physical model
</commit_message>
<xml_diff>
--- a/Documentation/Home_Automation_RMM.xlsx
+++ b/Documentation/Home_Automation_RMM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="21480" windowHeight="16460"/>
+    <workbookView xWindow="4340" yWindow="0" windowWidth="23300" windowHeight="20460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -393,7 +393,82 @@
         </r>
       </text>
     </comment>
-    <comment ref="M11" authorId="0">
+    <comment ref="F11" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Jheryl Lezama:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">1) The cost to correct (in hours) relates to the time it would take to solder up the physical wires.
+2) Time is based on a 8 hour work day.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J11" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Jheryl Lezama:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>1) The cost to correct (in hours) relates to the time it would take to transfer the wiring from the breadboard to hard soldering.
+2) Time is based on a 8 hour work day.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K11" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jheryl Lezama:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Despite the Mitigation Plan there is still a 10% risk that the issues with the wiring may persist.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -422,7 +497,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Number</t>
   </si>
@@ -512,6 +587,15 @@
   </si>
   <si>
     <t>1. Install a cooling fan in the attic to reduce the heat build-up in addition to a heat extractor vent that can help cool the system.</t>
+  </si>
+  <si>
+    <t>R-005</t>
+  </si>
+  <si>
+    <t>Due to the design of the physical model, their exists the hazard of loose wiring leading to shorts in the circuit.</t>
+  </si>
+  <si>
+    <t>1. Take the wires oiff of the breadboard and actually solder the wires into the model.</t>
   </si>
 </sst>
 </file>
@@ -1153,13 +1237,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y139"/>
+  <dimension ref="A1:Y140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
+      <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1529,7 +1613,7 @@
       <c r="J9" s="13">
         <v>16</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="13">
         <v>0.1</v>
       </c>
       <c r="L9" s="4">
@@ -1555,15 +1639,15 @@
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="H10" s="6"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="J10" s="13"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="5"/>
@@ -1580,76 +1664,103 @@
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
     </row>
-    <row r="11" spans="1:25" s="11" customFormat="1" ht="25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8" t="s">
+    <row r="11" spans="1:25" ht="61">
+      <c r="A11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="6">
+        <v>43177</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2</v>
+      </c>
+      <c r="G11" s="13">
+        <v>5</v>
+      </c>
+      <c r="H11" s="6">
+        <v>43187</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="4">
+        <v>2</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="M11" s="5">
+        <f>K11+L11</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+    </row>
+    <row r="12" spans="1:25" s="11" customFormat="1" ht="25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F12" s="9">
         <f>SUM(F3:F7)</f>
         <v>40.5</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G12" s="9">
         <f>SUM(G3:G7)</f>
         <v>20.125</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9">
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9">
         <f>SUM(J3:J7)</f>
         <v>25</v>
       </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9">
+      <c r="K12" s="9"/>
+      <c r="L12" s="9">
         <f>SUM(L3:L7)</f>
         <v>5.65</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M12" s="9">
         <f>SUM(M3:M7)</f>
         <v>30.65</v>
       </c>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="10"/>
-      <c r="X11" s="10"/>
-      <c r="Y11" s="10"/>
-    </row>
-    <row r="12" spans="1:25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="5"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="5"/>
-      <c r="Y12" s="5"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
     </row>
     <row r="13" spans="1:25">
       <c r="A13" s="4"/>
@@ -4757,18 +4868,18 @@
       <c r="Y127" s="5"/>
     </row>
     <row r="128" spans="1:25">
-      <c r="A128" s="5"/>
-      <c r="B128" s="5"/>
-      <c r="C128" s="5"/>
-      <c r="D128" s="5"/>
-      <c r="E128" s="5"/>
-      <c r="F128" s="5"/>
-      <c r="G128" s="5"/>
-      <c r="H128" s="5"/>
-      <c r="I128" s="5"/>
-      <c r="J128" s="5"/>
-      <c r="K128" s="5"/>
-      <c r="L128" s="5"/>
+      <c r="A128" s="4"/>
+      <c r="B128" s="4"/>
+      <c r="C128" s="4"/>
+      <c r="D128" s="4"/>
+      <c r="E128" s="4"/>
+      <c r="F128" s="4"/>
+      <c r="G128" s="4"/>
+      <c r="H128" s="4"/>
+      <c r="I128" s="4"/>
+      <c r="J128" s="4"/>
+      <c r="K128" s="4"/>
+      <c r="L128" s="4"/>
       <c r="M128" s="5"/>
       <c r="N128" s="5"/>
       <c r="O128" s="5"/>
@@ -5080,6 +5191,33 @@
       <c r="X139" s="5"/>
       <c r="Y139" s="5"/>
     </row>
+    <row r="140" spans="1:25">
+      <c r="A140" s="5"/>
+      <c r="B140" s="5"/>
+      <c r="C140" s="5"/>
+      <c r="D140" s="5"/>
+      <c r="E140" s="5"/>
+      <c r="F140" s="5"/>
+      <c r="G140" s="5"/>
+      <c r="H140" s="5"/>
+      <c r="I140" s="5"/>
+      <c r="J140" s="5"/>
+      <c r="K140" s="5"/>
+      <c r="L140" s="5"/>
+      <c r="M140" s="5"/>
+      <c r="N140" s="5"/>
+      <c r="O140" s="5"/>
+      <c r="P140" s="5"/>
+      <c r="Q140" s="5"/>
+      <c r="R140" s="5"/>
+      <c r="S140" s="5"/>
+      <c r="T140" s="5"/>
+      <c r="U140" s="5"/>
+      <c r="V140" s="5"/>
+      <c r="W140" s="5"/>
+      <c r="X140" s="5"/>
+      <c r="Y140" s="5"/>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>

</xml_diff>